<commit_message>
Fixing a bug in the spreadsheet
It had a hard-coded value where it should have had a reference.
</commit_message>
<xml_diff>
--- a/public/budget-template.xlsx
+++ b/public/budget-template.xlsx
@@ -4925,36 +4925,36 @@
         <v>0.4402586303640335</v>
       </c>
       <c r="D6" s="104">
-        <f>156000*103%</f>
-        <v>160680</v>
+        <f>B6*103%</f>
+        <v>105060</v>
       </c>
       <c r="E6" s="17">
         <f>D6/$D$34</f>
-        <v>0.5353492780880954</v>
+        <v>0.4396579322350952</v>
       </c>
       <c r="F6" s="105">
         <f>D6*103%</f>
-        <v>165500.4</v>
+        <v>108211.8</v>
       </c>
       <c r="G6" s="17">
         <f>F6/$F$34</f>
-        <v>0.5538066999439553</v>
+        <v>0.45886679173593</v>
       </c>
       <c r="H6" s="104">
         <f>F6*103%</f>
-        <v>170465.412</v>
+        <v>111458.154</v>
       </c>
       <c r="I6" s="17">
         <f>H6/$H$34</f>
-        <v>0.5619227470701921</v>
+        <v>0.4674219871593259</v>
       </c>
       <c r="J6" s="105">
         <f>H6*103%</f>
-        <v>175579.37436</v>
+        <v>114801.89862</v>
       </c>
       <c r="K6" s="17">
         <f>J6/$J$34</f>
-        <v>0.5650449981602538</v>
+        <v>0.4707311234590036</v>
       </c>
       <c r="L6" s="106"/>
       <c r="M6" t="s" s="107">
@@ -4980,28 +4980,28 @@
       </c>
       <c r="E7" s="17">
         <f>D7/$D$34</f>
-        <v>0.01665886476500172</v>
+        <v>0.02092413536241649</v>
       </c>
       <c r="F7" s="105">
         <v>5000</v>
       </c>
       <c r="G7" s="17">
         <f>F7/$F$34</f>
-        <v>0.01673127980186016</v>
+        <v>0.02120225297684402</v>
       </c>
       <c r="H7" s="104">
         <v>5000</v>
       </c>
       <c r="I7" s="17">
         <f>H7/$H$34</f>
-        <v>0.01648201651224684</v>
+        <v>0.02096849671309493</v>
       </c>
       <c r="J7" s="105">
         <v>5000</v>
       </c>
       <c r="K7" s="17">
         <f>J7/$J$34</f>
-        <v>0.01609087058829903</v>
+        <v>0.02050188756098656</v>
       </c>
       <c r="L7" s="106"/>
       <c r="M7" s="93"/>
@@ -5025,28 +5025,28 @@
       </c>
       <c r="E8" s="17">
         <f>D8/$D$34</f>
-        <v>0.01199438263080124</v>
+        <v>0.01506537746093987</v>
       </c>
       <c r="F8" s="104">
         <v>3600</v>
       </c>
       <c r="G8" s="17">
         <f>F8/$F$34</f>
-        <v>0.01204652145733931</v>
+        <v>0.01526562214332769</v>
       </c>
       <c r="H8" s="104">
         <v>3600</v>
       </c>
       <c r="I8" s="17">
         <f>H8/$H$34</f>
-        <v>0.01186705188881772</v>
+        <v>0.01509731763342835</v>
       </c>
       <c r="J8" s="104">
         <v>3600</v>
       </c>
       <c r="K8" s="17">
         <f>J8/$J$34</f>
-        <v>0.0115854268235753</v>
+        <v>0.01476135904391032</v>
       </c>
       <c r="L8" s="106"/>
       <c r="M8" s="3"/>
@@ -5070,28 +5070,28 @@
       </c>
       <c r="E9" s="109">
         <f>D9/$D$34</f>
-        <v>0.01665886476500172</v>
+        <v>0.02092413536241649</v>
       </c>
       <c r="F9" s="108">
         <v>5000</v>
       </c>
       <c r="G9" s="109">
         <f>F9/$F$34</f>
-        <v>0.01673127980186016</v>
+        <v>0.02120225297684402</v>
       </c>
       <c r="H9" s="108">
         <v>5000</v>
       </c>
       <c r="I9" s="109">
         <f>H9/$H$34</f>
-        <v>0.01648201651224684</v>
+        <v>0.02096849671309493</v>
       </c>
       <c r="J9" s="108">
         <v>5000</v>
       </c>
       <c r="K9" s="109">
         <f>J9/$J$34</f>
-        <v>0.01609087058829903</v>
+        <v>0.02050188756098656</v>
       </c>
       <c r="L9" s="106"/>
       <c r="M9" s="3"/>
@@ -5113,35 +5113,35 @@
       </c>
       <c r="D10" s="110">
         <f>D6+D8+D9+D7</f>
-        <v>174280</v>
+        <v>118660</v>
       </c>
       <c r="E10" s="111">
         <f>D10/$D$34</f>
-        <v>0.5806613902489001</v>
+        <v>0.4965715804208681</v>
       </c>
       <c r="F10" s="110">
         <f>F6+F8+F9+F7</f>
-        <v>179100.4</v>
+        <v>121811.8</v>
       </c>
       <c r="G10" s="111">
         <f>F10/$F$34</f>
-        <v>0.5993157810050149</v>
+        <v>0.5165369198329457</v>
       </c>
       <c r="H10" s="110">
         <f>H6+H8+H9+H7</f>
-        <v>184065.412</v>
+        <v>125058.154</v>
       </c>
       <c r="I10" s="111">
         <f>H10/$H$34</f>
-        <v>0.6067538319835034</v>
+        <v>0.524456298218944</v>
       </c>
       <c r="J10" s="110">
         <f>J6+J8+J9+J7</f>
-        <v>189179.37436</v>
+        <v>128401.89862</v>
       </c>
       <c r="K10" s="111">
         <f>J10/$J$34</f>
-        <v>0.6088121661604272</v>
+        <v>0.5264962576248871</v>
       </c>
       <c r="L10" s="106"/>
       <c r="M10" s="3"/>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="E12" s="17">
         <f>D12/$D$34</f>
-        <v>0.1235421410972528</v>
+        <v>0.1551733878476807</v>
       </c>
       <c r="F12" s="104">
         <f>D12*103%</f>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="G12" s="17">
         <f>F12/$F$34</f>
-        <v>0.1278015461409128</v>
+        <v>0.1619529853185635</v>
       </c>
       <c r="H12" s="112">
         <f>F12*103%</f>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="I12" s="17">
         <f>H12/$H$34</f>
-        <v>0.1296744800931212</v>
+        <v>0.1649724660562327</v>
       </c>
       <c r="J12" s="104">
         <f>H12*103%</f>
@@ -5211,7 +5211,7 @@
       </c>
       <c r="K12" s="17">
         <f>J12/$J$34</f>
-        <v>0.1303949995754432</v>
+        <v>0.1661403965149425</v>
       </c>
       <c r="L12" s="106"/>
       <c r="M12" t="s" s="107">
@@ -5237,28 +5237,28 @@
       </c>
       <c r="E13" s="17">
         <f>D13/$D$34</f>
-        <v>0.008329432382500862</v>
+        <v>0.01046206768120824</v>
       </c>
       <c r="F13" s="104">
         <v>2500</v>
       </c>
       <c r="G13" s="17">
         <f>F13/$F$34</f>
-        <v>0.008365639900930078</v>
+        <v>0.01060112648842201</v>
       </c>
       <c r="H13" s="104">
         <v>2600</v>
       </c>
       <c r="I13" s="17">
         <f>H13/$H$34</f>
-        <v>0.008570648586368355</v>
+        <v>0.01090361829080937</v>
       </c>
       <c r="J13" s="104">
         <v>2600</v>
       </c>
       <c r="K13" s="17">
         <f>J13/$J$34</f>
-        <v>0.008367252705915495</v>
+        <v>0.01066098153171301</v>
       </c>
       <c r="L13" s="106"/>
       <c r="M13" s="3"/>
@@ -5282,28 +5282,28 @@
       </c>
       <c r="E14" s="17">
         <f>D14/$D$34</f>
-        <v>0.008329432382500862</v>
+        <v>0.01046206768120824</v>
       </c>
       <c r="F14" s="104">
         <v>2500</v>
       </c>
       <c r="G14" s="17">
         <f>F14/$F$34</f>
-        <v>0.008365639900930078</v>
+        <v>0.01060112648842201</v>
       </c>
       <c r="H14" s="104">
         <v>2500</v>
       </c>
       <c r="I14" s="17">
         <f>H14/$H$34</f>
-        <v>0.008241008256123419</v>
+        <v>0.01048424835654747</v>
       </c>
       <c r="J14" s="104">
         <v>2500</v>
       </c>
       <c r="K14" s="17">
         <f>J14/$J$34</f>
-        <v>0.008045435294149516</v>
+        <v>0.01025094378049328</v>
       </c>
       <c r="L14" s="106"/>
       <c r="M14" s="3"/>
@@ -5327,28 +5327,28 @@
       </c>
       <c r="E15" s="109">
         <f>D15/$D$34</f>
-        <v>0.01099485074490114</v>
+        <v>0.01380992933919488</v>
       </c>
       <c r="F15" s="108">
         <v>3300</v>
       </c>
       <c r="G15" s="109">
         <f>F15/$F$34</f>
-        <v>0.0110426446692277</v>
+        <v>0.01399348696471705</v>
       </c>
       <c r="H15" s="108">
         <v>3300</v>
       </c>
       <c r="I15" s="109">
         <f>H15/$H$34</f>
-        <v>0.01087813089808291</v>
+        <v>0.01383920783064266</v>
       </c>
       <c r="J15" s="108">
         <v>3300</v>
       </c>
       <c r="K15" s="109">
         <f>J15/$J$34</f>
-        <v>0.01061997458827736</v>
+        <v>0.01353124579025113</v>
       </c>
       <c r="L15" s="106"/>
       <c r="M15" s="3"/>
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E16" s="111">
         <f>D16/$D$34</f>
-        <v>0.1511958566071556</v>
+        <v>0.189907452549292</v>
       </c>
       <c r="F16" s="110">
         <f>SUM(F12:F15)</f>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="G16" s="111">
         <f>F16/$F$34</f>
-        <v>0.1555754706120006</v>
+        <v>0.1971487252601246</v>
       </c>
       <c r="H16" s="110">
         <f>SUM(H12:H15)</f>
@@ -5390,7 +5390,7 @@
       </c>
       <c r="I16" s="111">
         <f>H16/$H$34</f>
-        <v>0.1573642678336959</v>
+        <v>0.2001995405342321</v>
       </c>
       <c r="J16" s="110">
         <f>SUM(J12:J15)</f>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="K16" s="111">
         <f>J16/$J$34</f>
-        <v>0.1574276621637856</v>
+        <v>0.2005835676173999</v>
       </c>
       <c r="L16" s="106"/>
       <c r="M16" s="3"/>
@@ -5422,28 +5422,28 @@
       </c>
       <c r="E17" s="21">
         <f>D17/$D$34</f>
-        <v>0.04997659429500517</v>
+        <v>0.06277240608724946</v>
       </c>
       <c r="F17" s="113">
         <v>7500</v>
       </c>
       <c r="G17" s="21">
         <f>F17/$F$34</f>
-        <v>0.02509691970279023</v>
+        <v>0.03180337946526603</v>
       </c>
       <c r="H17" s="113">
         <v>5000</v>
       </c>
       <c r="I17" s="21">
         <f>H17/$H$34</f>
-        <v>0.01648201651224684</v>
+        <v>0.02096849671309493</v>
       </c>
       <c r="J17" s="113">
         <v>5000</v>
       </c>
       <c r="K17" s="21">
         <f>J17/$J$34</f>
-        <v>0.01609087058829903</v>
+        <v>0.02050188756098656</v>
       </c>
       <c r="L17" s="106"/>
       <c r="M17" t="s" s="107">
@@ -5469,28 +5469,28 @@
       </c>
       <c r="E18" s="21">
         <f>D18/$D$34</f>
-        <v>0.0666354590600069</v>
+        <v>0.08369654144966594</v>
       </c>
       <c r="F18" s="113">
         <v>20000</v>
       </c>
       <c r="G18" s="21">
         <f>F18/$F$34</f>
-        <v>0.06692511920744063</v>
+        <v>0.08480901190737608</v>
       </c>
       <c r="H18" s="113">
         <v>20000</v>
       </c>
       <c r="I18" s="21">
         <f>H18/$H$34</f>
-        <v>0.06592806604898735</v>
+        <v>0.08387398685237973</v>
       </c>
       <c r="J18" s="113">
         <v>20000</v>
       </c>
       <c r="K18" s="21">
         <f>J18/$J$34</f>
-        <v>0.06436348235319612</v>
+        <v>0.08200755024394624</v>
       </c>
       <c r="L18" s="106"/>
       <c r="M18" s="3"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="E20" s="17">
         <f>D20/$D$34</f>
-        <v>0.002059035684954213</v>
+        <v>0.002586223130794678</v>
       </c>
       <c r="F20" s="105">
         <f>D20*103%</f>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="G20" s="17">
         <f>F20/$F$34</f>
-        <v>0.002130025769015212</v>
+        <v>0.002699216421976059</v>
       </c>
       <c r="H20" s="104">
         <f>F20*103%</f>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="I20" s="17">
         <f>H20/$H$34</f>
-        <v>0.002161241334885354</v>
+        <v>0.002749541100937211</v>
       </c>
       <c r="J20" s="105">
         <f>H20*103%</f>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="K20" s="17">
         <f>J20/$J$34</f>
-        <v>0.002173249992924053</v>
+        <v>0.002769006608582374</v>
       </c>
       <c r="L20" s="106"/>
       <c r="M20" s="3"/>
@@ -5584,7 +5584,7 @@
       </c>
       <c r="E21" s="17">
         <f>D21/$D$34</f>
-        <v>0.0005147589212385532</v>
+        <v>0.0006465557826986695</v>
       </c>
       <c r="F21" s="105">
         <f>D21*103%</f>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="G21" s="17">
         <f>F21/$F$34</f>
-        <v>0.0005325064422538031</v>
+        <v>0.0006748041054940147</v>
       </c>
       <c r="H21" s="104">
         <f>F21*103%</f>
@@ -5600,7 +5600,7 @@
       </c>
       <c r="I21" s="17">
         <f>H21/$H$34</f>
-        <v>0.0005403103337213385</v>
+        <v>0.0006873852752343027</v>
       </c>
       <c r="J21" s="105">
         <f>H21*103%</f>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="K21" s="17">
         <f>J21/$J$34</f>
-        <v>0.0005433124982310132</v>
+        <v>0.0006922516521455936</v>
       </c>
       <c r="L21" s="106"/>
       <c r="M21" s="3"/>
@@ -5633,7 +5633,7 @@
       </c>
       <c r="E22" s="17">
         <f>D22/$D$34</f>
-        <v>0.01801656224334936</v>
+        <v>0.02262945239445343</v>
       </c>
       <c r="F22" s="105">
         <f>D22*103%</f>
@@ -5641,7 +5641,7 @@
       </c>
       <c r="G22" s="17">
         <f>F22/$F$34</f>
-        <v>0.01863772547888311</v>
+        <v>0.02361814369229051</v>
       </c>
       <c r="H22" s="104">
         <f>F22*103%</f>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="I22" s="17">
         <f>H22/$H$34</f>
-        <v>0.01891086168024685</v>
+        <v>0.0240584846332006</v>
       </c>
       <c r="J22" s="105">
         <f>H22*103%</f>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="K22" s="17">
         <f>J22/$J$34</f>
-        <v>0.01901593743808547</v>
+        <v>0.02422880782509578</v>
       </c>
       <c r="L22" s="106"/>
       <c r="M22" s="3"/>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="E23" s="17">
         <f>D23/$D$34</f>
-        <v>0.0003431726141590355</v>
+        <v>0.0004310371884657796</v>
       </c>
       <c r="F23" s="105">
         <f>D23*103%</f>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="G23" s="17">
         <f>F23/$F$34</f>
-        <v>0.0003550042948358688</v>
+        <v>0.0004498694036626765</v>
       </c>
       <c r="H23" s="104">
         <f>F23*103%</f>
@@ -5698,7 +5698,7 @@
       </c>
       <c r="I23" s="17">
         <f>H23/$H$34</f>
-        <v>0.000360206889147559</v>
+        <v>0.0004582568501562018</v>
       </c>
       <c r="J23" s="105">
         <f>H23*103%</f>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="K23" s="17">
         <f>J23/$J$34</f>
-        <v>0.0003622083321540088</v>
+        <v>0.0004615011014303957</v>
       </c>
       <c r="L23" s="106"/>
       <c r="M23" s="3"/>
@@ -5731,7 +5731,7 @@
       </c>
       <c r="E24" s="17">
         <f>D24/$D$34</f>
-        <v>0.000686345228318071</v>
+        <v>0.0008620743769315592</v>
       </c>
       <c r="F24" s="105">
         <f>D24*103%</f>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="G24" s="17">
         <f>F24/$F$34</f>
-        <v>0.0007100085896717376</v>
+        <v>0.0008997388073253529</v>
       </c>
       <c r="H24" s="104">
         <f>F24*103%</f>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="I24" s="17">
         <f>H24/$H$34</f>
-        <v>0.000720413778295118</v>
+        <v>0.0009165137003124035</v>
       </c>
       <c r="J24" s="105">
         <f>H24*103%</f>
@@ -5755,7 +5755,7 @@
       </c>
       <c r="K24" s="17">
         <f>J24/$J$34</f>
-        <v>0.0007244166643080176</v>
+        <v>0.0009230022028607914</v>
       </c>
       <c r="L24" s="106"/>
       <c r="M24" s="3"/>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="E25" s="17">
         <f>D25/$D$34</f>
-        <v>0.01715863070795177</v>
+        <v>0.02155185942328898</v>
       </c>
       <c r="F25" s="105">
         <f>D25*103%</f>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="G25" s="17">
         <f>F25/$F$34</f>
-        <v>0.01775021474179344</v>
+        <v>0.02249347018313382</v>
       </c>
       <c r="H25" s="104">
         <f>F25*103%</f>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="I25" s="17">
         <f>H25/$H$34</f>
-        <v>0.01801034445737795</v>
+        <v>0.02291284250781009</v>
       </c>
       <c r="J25" s="105">
         <f>H25*103%</f>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="K25" s="17">
         <f>J25/$J$34</f>
-        <v>0.01811041660770044</v>
+        <v>0.02307505507151979</v>
       </c>
       <c r="L25" s="106"/>
       <c r="M25" s="3"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="E26" s="109">
         <f>D26/$D$34</f>
-        <v>0.004118071369908426</v>
+        <v>0.005172446261589356</v>
       </c>
       <c r="F26" s="114">
         <f>D26*103%</f>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="G26" s="109">
         <f>F26/$F$34</f>
-        <v>0.004260051538030425</v>
+        <v>0.005398432843952117</v>
       </c>
       <c r="H26" s="108">
         <f>F26*103%</f>
@@ -5845,7 +5845,7 @@
       </c>
       <c r="I26" s="109">
         <f>H26/$H$34</f>
-        <v>0.004322482669770708</v>
+        <v>0.005499082201874421</v>
       </c>
       <c r="J26" s="114">
         <f>H26*103%</f>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="K26" s="109">
         <f>J26/$J$34</f>
-        <v>0.004346499985848106</v>
+        <v>0.005538013217164748</v>
       </c>
       <c r="L26" s="106"/>
       <c r="M26" s="3"/>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="E27" s="115">
         <f>D27/$D$34</f>
-        <v>0.04289657676987944</v>
+        <v>0.05387964855822245</v>
       </c>
       <c r="F27" s="110">
         <f>SUM(F20:F26)</f>
@@ -5887,7 +5887,7 @@
       </c>
       <c r="G27" s="115">
         <f>F27/$F$34</f>
-        <v>0.0443755368544836</v>
+        <v>0.05623367545783456</v>
       </c>
       <c r="H27" s="110">
         <f>SUM(H20:H26)</f>
@@ -5895,7 +5895,7 @@
       </c>
       <c r="I27" s="115">
         <f>H27/$H$34</f>
-        <v>0.04502586114344487</v>
+        <v>0.05728210626952523</v>
       </c>
       <c r="J27" s="110">
         <f>SUM(J20:J26)</f>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="K27" s="115">
         <f>J27/$J$34</f>
-        <v>0.0452760415192511</v>
+        <v>0.05768763767879947</v>
       </c>
       <c r="L27" s="106"/>
       <c r="M27" t="s" s="107">
@@ -5929,28 +5929,28 @@
       </c>
       <c r="E28" s="17">
         <f>D28/$D$34</f>
-        <v>0.0009995318859001034</v>
+        <v>0.001255448121744989</v>
       </c>
       <c r="F28" s="113">
         <v>300</v>
       </c>
       <c r="G28" s="17">
         <f>F28/$F$34</f>
-        <v>0.001003876788111609</v>
+        <v>0.001272135178610641</v>
       </c>
       <c r="H28" s="113">
         <v>300</v>
       </c>
       <c r="I28" s="17">
         <f>H28/$H$34</f>
-        <v>0.0009889209907348103</v>
+        <v>0.001258109802785696</v>
       </c>
       <c r="J28" s="113">
         <v>300</v>
       </c>
       <c r="K28" s="17">
         <f>J28/$J$34</f>
-        <v>0.0009654522352979418</v>
+        <v>0.001230113253659194</v>
       </c>
       <c r="L28" s="106"/>
       <c r="M28" s="3"/>
@@ -5974,28 +5974,28 @@
       </c>
       <c r="E29" s="17">
         <f>D29/$D$34</f>
-        <v>0.0008329432382500862</v>
+        <v>0.001046206768120824</v>
       </c>
       <c r="F29" s="113">
         <v>250</v>
       </c>
       <c r="G29" s="17">
         <f>F29/$F$34</f>
-        <v>0.0008365639900930078</v>
+        <v>0.001060112648842201</v>
       </c>
       <c r="H29" s="113">
         <v>250</v>
       </c>
       <c r="I29" s="17">
         <f>H29/$H$34</f>
-        <v>0.0008241008256123419</v>
+        <v>0.001048424835654747</v>
       </c>
       <c r="J29" s="113">
         <v>250</v>
       </c>
       <c r="K29" s="17">
         <f>J29/$J$34</f>
-        <v>0.0008045435294149515</v>
+        <v>0.001025094378049328</v>
       </c>
       <c r="L29" s="106"/>
       <c r="M29" s="3"/>
@@ -6019,28 +6019,28 @@
       </c>
       <c r="E30" s="17">
         <f>D30/$D$34</f>
-        <v>0.002398876526160248</v>
+        <v>0.003013075492187974</v>
       </c>
       <c r="F30" s="113">
         <v>720</v>
       </c>
       <c r="G30" s="17">
         <f>F30/$F$34</f>
-        <v>0.002409304291467863</v>
+        <v>0.003053124428665539</v>
       </c>
       <c r="H30" s="113">
         <v>720</v>
       </c>
       <c r="I30" s="17">
         <f>H30/$H$34</f>
-        <v>0.002373410377763545</v>
+        <v>0.00301946352668567</v>
       </c>
       <c r="J30" s="113">
         <v>720</v>
       </c>
       <c r="K30" s="17">
         <f>J30/$J$34</f>
-        <v>0.00231708536471506</v>
+        <v>0.002952271808782065</v>
       </c>
       <c r="L30" s="106"/>
       <c r="M30" s="3"/>
@@ -6064,28 +6064,28 @@
       </c>
       <c r="E31" s="17">
         <f>D31/$D$34</f>
-        <v>0.0134936804596514</v>
+        <v>0.01694854964355735</v>
       </c>
       <c r="F31" s="113">
         <v>4050</v>
       </c>
       <c r="G31" s="17">
         <f>F31/$F$34</f>
-        <v>0.01355233663950673</v>
+        <v>0.01717382491124366</v>
       </c>
       <c r="H31" s="113">
         <v>4050</v>
       </c>
       <c r="I31" s="17">
         <f>H31/$H$34</f>
-        <v>0.01335043337491994</v>
+        <v>0.0169844823376069</v>
       </c>
       <c r="J31" s="113">
         <v>4050</v>
       </c>
       <c r="K31" s="17">
         <f>J31/$J$34</f>
-        <v>0.01303360517652221</v>
+        <v>0.01660652892439911</v>
       </c>
       <c r="L31" s="106"/>
       <c r="M31" s="3"/>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="D33" s="117">
         <f>10%*(SUM(D27:D32)+D17+D16+D10+D18)</f>
-        <v>27285.5</v>
+        <v>21723.5</v>
       </c>
       <c r="E33" s="118">
         <f>D33/$D$34</f>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="F33" s="117">
         <f>10%*(SUM(F27:F32)+F17+F16+F10+F18)</f>
-        <v>27167.405</v>
+        <v>21438.545</v>
       </c>
       <c r="G33" s="118">
         <f>F33/$F$34</f>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="H33" s="117">
         <f>10%*(SUM(H27:H32)+H17+H16+H10+H18)</f>
-        <v>27578.267150000007</v>
+        <v>21677.54135</v>
       </c>
       <c r="I33" s="118">
         <f>H33/$H$34</f>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="J33" s="117">
         <f>10%*(SUM(J27:J32)+J17+J16+J10+J18)</f>
-        <v>28248.6551645</v>
+        <v>22170.907590500006</v>
       </c>
       <c r="K33" s="118">
         <f>J33/$J$34</f>
@@ -6204,15 +6204,15 @@
       </c>
       <c r="D34" s="119">
         <f>D10+D16+D17+D27+D28+D30+D29+D31+D32+D33+D18</f>
-        <v>300140.5</v>
+        <v>238958.5</v>
       </c>
       <c r="E34" s="120">
         <f>E10+E16+E17+E27+E28+E30+E29+E31+E32+E33+E18</f>
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F34" s="119">
         <f>F10+F16+F17+F27+F28+F30+F29+F31+F32+F33+F18</f>
-        <v>298841.455</v>
+        <v>235823.995</v>
       </c>
       <c r="G34" s="120">
         <f>G10+G16+G17+G27+G28+G30+G29+G31+G32+G33+G18</f>
@@ -6220,19 +6220,19 @@
       </c>
       <c r="H34" s="119">
         <f>H10+H16+H17+H27+H28+H30+H29+H31+H32+H33+H18</f>
-        <v>303360.93865</v>
+        <v>238452.95485</v>
       </c>
       <c r="I34" s="120">
         <f>I10+I16+I17+I27+I28+I30+I29+I31+I32+I33+I18</f>
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="J34" s="119">
         <f>J10+J16+J17+J27+J28+J30+J29+J31+J32+J33+J18</f>
-        <v>310735.2068095</v>
+        <v>243879.9834955001</v>
       </c>
       <c r="K34" s="120">
         <f>K10+K16+K17+K27+K28+K30+K29+K31+K32+K33+K18</f>
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="L34" s="106"/>
       <c r="M34" s="3"/>

</xml_diff>